<commit_message>
Do not use this branch
</commit_message>
<xml_diff>
--- a/AAE 560 Air Taxi Model/+airtaxi/Inputs.xlsx
+++ b/AAE 560 Air Taxi Model/+airtaxi/Inputs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Documents\GitHub\SoS12\AAE 560 Air Taxi Model\+airtaxi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmyers\Documents\GitHub\SoS12\AAE 560 Air Taxi Model\+airtaxi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B61117-199A-4DB2-98EC-2AD4CC4C855C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{1F9822AC-5DDB-4CA4-A664-983A8488F4F0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2832" yWindow="0" windowWidth="22692" windowHeight="8748" xr2:uid="{D283E0F8-1F52-4946-9F02-CCA289FF9208}"/>
+    <workbookView xWindow="2835" yWindow="0" windowWidth="22695" windowHeight="8745" xr2:uid="{D283E0F8-1F52-4946-9F02-CCA289FF9208}"/>
   </bookViews>
   <sheets>
     <sheet name="runs" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
   <si>
     <t>Visibility</t>
   </si>
@@ -71,18 +71,6 @@
   </si>
   <si>
     <t>Stop Run ID (inclusive)</t>
-  </si>
-  <si>
-    <t>config2</t>
-  </si>
-  <si>
-    <t>config3</t>
-  </si>
-  <si>
-    <t>config4</t>
-  </si>
-  <si>
-    <t>config5</t>
   </si>
 </sst>
 </file>
@@ -440,15 +428,15 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -456,15 +444,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
       <c r="B2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -479,25 +467,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD319FC3-F5A0-442C-9F04-E5E568694E63}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -532,12 +518,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -567,15 +553,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
         <v>0</v>
-      </c>
-      <c r="C3">
-        <v>20</v>
       </c>
       <c r="D3">
         <v>0.9</v>
@@ -599,10 +585,10 @@
         <v>500</v>
       </c>
       <c r="K3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -610,7 +596,7 @@
         <v>10</v>
       </c>
       <c r="C4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <v>0.8</v>
@@ -634,18 +620,18 @@
         <v>500</v>
       </c>
       <c r="K4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C5">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <v>0.7</v>
@@ -669,18 +655,18 @@
         <v>500</v>
       </c>
       <c r="K5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6">
         <v>0</v>
-      </c>
-      <c r="C6">
-        <v>30</v>
       </c>
       <c r="D6">
         <v>0.6</v>
@@ -704,7 +690,357 @@
         <v>500</v>
       </c>
       <c r="K6" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>270</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <v>3</v>
+      </c>
+      <c r="I7">
+        <v>5</v>
+      </c>
+      <c r="J7">
+        <v>500</v>
+      </c>
+      <c r="K7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>0.9</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>270</v>
+      </c>
+      <c r="G8">
+        <v>5</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+      <c r="I8">
+        <v>5</v>
+      </c>
+      <c r="J8">
+        <v>500</v>
+      </c>
+      <c r="K8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>0.8</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>270</v>
+      </c>
+      <c r="G9">
+        <v>5</v>
+      </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
+      <c r="I9">
+        <v>5</v>
+      </c>
+      <c r="J9">
+        <v>500</v>
+      </c>
+      <c r="K9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>0.7</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <v>270</v>
+      </c>
+      <c r="G10">
+        <v>5</v>
+      </c>
+      <c r="H10">
+        <v>3</v>
+      </c>
+      <c r="I10">
+        <v>5</v>
+      </c>
+      <c r="J10">
+        <v>500</v>
+      </c>
+      <c r="K10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>0.6</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <v>270</v>
+      </c>
+      <c r="G11">
+        <v>5</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+      <c r="I11">
+        <v>5</v>
+      </c>
+      <c r="J11">
+        <v>500</v>
+      </c>
+      <c r="K11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <v>270</v>
+      </c>
+      <c r="G12">
+        <v>5</v>
+      </c>
+      <c r="H12">
+        <v>3</v>
+      </c>
+      <c r="I12">
+        <v>5</v>
+      </c>
+      <c r="J12">
+        <v>500</v>
+      </c>
+      <c r="K12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>0.9</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+      <c r="F13">
+        <v>270</v>
+      </c>
+      <c r="G13">
+        <v>5</v>
+      </c>
+      <c r="H13">
+        <v>3</v>
+      </c>
+      <c r="I13">
+        <v>5</v>
+      </c>
+      <c r="J13">
+        <v>500</v>
+      </c>
+      <c r="K13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>0.8</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <v>270</v>
+      </c>
+      <c r="G14">
+        <v>5</v>
+      </c>
+      <c r="H14">
+        <v>3</v>
+      </c>
+      <c r="I14">
+        <v>5</v>
+      </c>
+      <c r="J14">
+        <v>500</v>
+      </c>
+      <c r="K14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>0.7</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>270</v>
+      </c>
+      <c r="G15">
+        <v>5</v>
+      </c>
+      <c r="H15">
+        <v>3</v>
+      </c>
+      <c r="I15">
+        <v>5</v>
+      </c>
+      <c r="J15">
+        <v>500</v>
+      </c>
+      <c r="K15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>0.6</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="F16">
+        <v>270</v>
+      </c>
+      <c r="G16">
+        <v>5</v>
+      </c>
+      <c r="H16">
+        <v>3</v>
+      </c>
+      <c r="I16">
+        <v>5</v>
+      </c>
+      <c r="J16">
+        <v>500</v>
+      </c>
+      <c r="K16" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Included a port check and removed waiting times
</commit_message>
<xml_diff>
--- a/AAE 560 Air Taxi Model/+airtaxi/Inputs.xlsx
+++ b/AAE 560 Air Taxi Model/+airtaxi/Inputs.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Documents\GitHub\SoS12\AAE 560 Air Taxi Model\+airtaxi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96E943F9-E6A8-4DC4-BC46-84E981F9C6A9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6426EAF1-90E2-4F27-90C3-B7BD745C9C0A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2832" yWindow="0" windowWidth="22692" windowHeight="8748" activeTab="1" xr2:uid="{D283E0F8-1F52-4946-9F02-CCA289FF9208}"/>
+    <workbookView xWindow="2832" yWindow="0" windowWidth="22692" windowHeight="8748" xr2:uid="{D283E0F8-1F52-4946-9F02-CCA289FF9208}"/>
   </bookViews>
   <sheets>
     <sheet name="runs" sheetId="2" r:id="rId1"/>
     <sheet name="params" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -439,7 +439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98028C58-071A-4E37-9E82-3C2AA620C0F8}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -469,7 +469,7 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>100</v>
+        <v>500</v>
       </c>
     </row>
   </sheetData>
@@ -481,7 +481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD319FC3-F5A0-442C-9F04-E5E568694E63}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Scaled speed by factor of 10
Will need to verify functionality
</commit_message>
<xml_diff>
--- a/AAE 560 Air Taxi Model/+airtaxi/Inputs.xlsx
+++ b/AAE 560 Air Taxi Model/+airtaxi/Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmyers\Documents\GitHub\SoS12\AAE 560 Air Taxi Model\+airtaxi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{1F9822AC-5DDB-4CA4-A664-983A8488F4F0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{688A2881-744C-4D9B-B572-952F4401DF18}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2835" yWindow="0" windowWidth="22695" windowHeight="8745" xr2:uid="{D283E0F8-1F52-4946-9F02-CCA289FF9208}"/>
+    <workbookView xWindow="3780" yWindow="0" windowWidth="22695" windowHeight="8745" activeTab="1" xr2:uid="{D283E0F8-1F52-4946-9F02-CCA289FF9208}"/>
   </bookViews>
   <sheets>
     <sheet name="runs" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
   <si>
     <t>Visibility</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>Stop Run ID (inclusive)</t>
+  </si>
+  <si>
+    <t>config5</t>
   </si>
 </sst>
 </file>
@@ -427,8 +430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98028C58-071A-4E37-9E82-3C2AA620C0F8}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,7 +452,7 @@
         <v>14</v>
       </c>
       <c r="B2">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -469,7 +472,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD319FC3-F5A0-442C-9F04-E5E568694E63}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -529,7 +534,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -550,7 +555,7 @@
         <v>500</v>
       </c>
       <c r="K2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Debugged collision and landing clearance algorithm
Still need to debug takeoff clearance
</commit_message>
<xml_diff>
--- a/AAE 560 Air Taxi Model/+airtaxi/Inputs.xlsx
+++ b/AAE 560 Air Taxi Model/+airtaxi/Inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Documents\GitHub\SoS12\AAE 560 Air Taxi Model\+airtaxi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6426EAF1-90E2-4F27-90C3-B7BD745C9C0A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62C9CEE-9910-43FE-B301-FCCBAA491597}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2832" yWindow="0" windowWidth="22692" windowHeight="8748" xr2:uid="{D283E0F8-1F52-4946-9F02-CCA289FF9208}"/>
   </bookViews>
@@ -453,7 +453,7 @@
         <v>13</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -461,7 +461,7 @@
         <v>14</v>
       </c>
       <c r="B2">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -469,7 +469,7 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>500</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -482,7 +482,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -683,7 +683,7 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6">
         <v>3</v>

</xml_diff>

<commit_message>
Tried to debug takeoff clearance
</commit_message>
<xml_diff>
--- a/AAE 560 Air Taxi Model/+airtaxi/Inputs.xlsx
+++ b/AAE 560 Air Taxi Model/+airtaxi/Inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Documents\GitHub\SoS12\AAE 560 Air Taxi Model\+airtaxi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62C9CEE-9910-43FE-B301-FCCBAA491597}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1EC6702-261B-4E8D-BDAE-ECD4054CD1EE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2832" yWindow="0" windowWidth="22692" windowHeight="8748" xr2:uid="{D283E0F8-1F52-4946-9F02-CCA289FF9208}"/>
   </bookViews>
@@ -453,7 +453,7 @@
         <v>13</v>
       </c>
       <c r="B1">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -461,7 +461,7 @@
         <v>14</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -469,7 +469,7 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>200</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Debugged clearance algorithm. Hooray!
</commit_message>
<xml_diff>
--- a/AAE 560 Air Taxi Model/+airtaxi/Inputs.xlsx
+++ b/AAE 560 Air Taxi Model/+airtaxi/Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Documents\GitHub\SoS12\AAE 560 Air Taxi Model\+airtaxi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1EC6702-261B-4E8D-BDAE-ECD4054CD1EE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{045D7FBE-BD6D-47ED-B774-D569222BF2EF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2832" yWindow="0" windowWidth="22692" windowHeight="8748" xr2:uid="{D283E0F8-1F52-4946-9F02-CCA289FF9208}"/>
+    <workbookView xWindow="2832" yWindow="0" windowWidth="22692" windowHeight="8748" activeTab="1" xr2:uid="{D283E0F8-1F52-4946-9F02-CCA289FF9208}"/>
   </bookViews>
   <sheets>
     <sheet name="runs" sheetId="2" r:id="rId1"/>
@@ -439,7 +439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98028C58-071A-4E37-9E82-3C2AA620C0F8}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -481,7 +481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD319FC3-F5A0-442C-9F04-E5E568694E63}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Cleaned up a couple items in clearance and collision algorithms
</commit_message>
<xml_diff>
--- a/AAE 560 Air Taxi Model/+airtaxi/Inputs.xlsx
+++ b/AAE 560 Air Taxi Model/+airtaxi/Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Documents\GitHub\SoS12\AAE 560 Air Taxi Model\+airtaxi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{045D7FBE-BD6D-47ED-B774-D569222BF2EF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9012600A-5FEA-4454-A369-6CB33386F83B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2832" yWindow="0" windowWidth="22692" windowHeight="8748" activeTab="1" xr2:uid="{D283E0F8-1F52-4946-9F02-CCA289FF9208}"/>
+    <workbookView xWindow="2832" yWindow="0" windowWidth="22692" windowHeight="8748" xr2:uid="{D283E0F8-1F52-4946-9F02-CCA289FF9208}"/>
   </bookViews>
   <sheets>
     <sheet name="runs" sheetId="2" r:id="rId1"/>
@@ -439,7 +439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98028C58-071A-4E37-9E82-3C2AA620C0F8}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -453,7 +453,7 @@
         <v>13</v>
       </c>
       <c r="B1">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -461,7 +461,7 @@
         <v>14</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -469,7 +469,7 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>150</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -481,8 +481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD319FC3-F5A0-442C-9F04-E5E568694E63}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -683,7 +683,7 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <v>3</v>

</xml_diff>

<commit_message>
Save before move - no change
</commit_message>
<xml_diff>
--- a/AAE 560 Air Taxi Model/+airtaxi/Inputs.xlsx
+++ b/AAE 560 Air Taxi Model/+airtaxi/Inputs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmyers\Documents\GitHub\SoS12\AAE 560 Air Taxi Model\+airtaxi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Documents\GitHub\SoS12\AAE 560 Air Taxi Model\+airtaxi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{688A2881-744C-4D9B-B572-952F4401DF18}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF71612-3BA7-47DF-8134-1DC8ED2E56AA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="0" windowWidth="22695" windowHeight="8745" activeTab="1" xr2:uid="{D283E0F8-1F52-4946-9F02-CCA289FF9208}"/>
+    <workbookView xWindow="3780" yWindow="0" windowWidth="22692" windowHeight="8748" activeTab="1" xr2:uid="{D283E0F8-1F52-4946-9F02-CCA289FF9208}"/>
   </bookViews>
   <sheets>
     <sheet name="runs" sheetId="2" r:id="rId1"/>
@@ -434,12 +434,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -447,7 +447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -455,7 +455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -473,22 +473,22 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -523,7 +523,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -558,7 +558,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -593,7 +593,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -628,7 +628,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -663,7 +663,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -698,7 +698,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -733,7 +733,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -768,7 +768,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -803,7 +803,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -838,7 +838,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -873,7 +873,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -908,7 +908,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -943,7 +943,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -978,7 +978,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1013,7 +1013,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
updated inputs and PortLocations
</commit_message>
<xml_diff>
--- a/AAE 560 Air Taxi Model/+airtaxi/Inputs.xlsx
+++ b/AAE 560 Air Taxi Model/+airtaxi/Inputs.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmyers\Documents\GitHub\SoS12\AAE 560 Air Taxi Model\+airtaxi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Documents\GitHub\SoS12\AAE 560 Air Taxi Model\+airtaxi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{688A2881-744C-4D9B-B572-952F4401DF18}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5411BE5-CF36-4C6E-982A-7CD81721CBE8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="0" windowWidth="22695" windowHeight="8745" activeTab="1" xr2:uid="{D283E0F8-1F52-4946-9F02-CCA289FF9208}"/>
+    <workbookView xWindow="2832" yWindow="0" windowWidth="22692" windowHeight="8748" activeTab="1" xr2:uid="{D283E0F8-1F52-4946-9F02-CCA289FF9208}"/>
   </bookViews>
   <sheets>
     <sheet name="runs" sheetId="2" r:id="rId1"/>
     <sheet name="params" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
   <si>
     <t>Visibility</t>
   </si>
@@ -71,6 +71,15 @@
   </si>
   <si>
     <t>Stop Run ID (inclusive)</t>
+  </si>
+  <si>
+    <t>config2</t>
+  </si>
+  <si>
+    <t>config3</t>
+  </si>
+  <si>
+    <t>config4</t>
   </si>
   <si>
     <t>config5</t>
@@ -434,12 +443,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -447,20 +456,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
       <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3">
-        <v>100</v>
+        <v>500</v>
       </c>
     </row>
   </sheetData>
@@ -473,22 +482,22 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="J2" sqref="J2:J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -523,7 +532,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -534,7 +543,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -552,18 +561,18 @@
         <v>5</v>
       </c>
       <c r="J2">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -587,18 +596,18 @@
         <v>5</v>
       </c>
       <c r="J3">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -622,18 +631,18 @@
         <v>5</v>
       </c>
       <c r="J4">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -657,24 +666,24 @@
         <v>5</v>
       </c>
       <c r="J5">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <v>3</v>
@@ -692,13 +701,13 @@
         <v>5</v>
       </c>
       <c r="J6">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -727,13 +736,13 @@
         <v>5</v>
       </c>
       <c r="J7">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -741,7 +750,7 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D8">
         <v>0.9</v>
@@ -762,13 +771,13 @@
         <v>5</v>
       </c>
       <c r="J8">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -776,7 +785,7 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D9">
         <v>0.8</v>
@@ -797,13 +806,13 @@
         <v>5</v>
       </c>
       <c r="J9">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -811,7 +820,7 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D10">
         <v>0.7</v>
@@ -832,13 +841,13 @@
         <v>5</v>
       </c>
       <c r="J10">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -846,10 +855,10 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D11">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="E11">
         <v>3</v>
@@ -867,21 +876,21 @@
         <v>5</v>
       </c>
       <c r="J11">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C12">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -902,21 +911,21 @@
         <v>5</v>
       </c>
       <c r="J12">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C13">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D13">
         <v>0.9</v>
@@ -937,21 +946,21 @@
         <v>5</v>
       </c>
       <c r="J13">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D14">
         <v>0.8</v>
@@ -972,21 +981,21 @@
         <v>5</v>
       </c>
       <c r="J14">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C15">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D15">
         <v>0.7</v>
@@ -1007,24 +1016,24 @@
         <v>5</v>
       </c>
       <c r="J15">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C16">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="D16">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="E16">
         <v>3</v>
@@ -1042,10 +1051,10 @@
         <v>5</v>
       </c>
       <c r="J16">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K16" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated VisualSA and Datalink Buffers
</commit_message>
<xml_diff>
--- a/AAE 560 Air Taxi Model/+airtaxi/Inputs.xlsx
+++ b/AAE 560 Air Taxi Model/+airtaxi/Inputs.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Documents\GitHub\SoS12\AAE 560 Air Taxi Model\+airtaxi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmyers\Documents\GitHub\SoS12\AAE 560 Air Taxi Model\+airtaxi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5411BE5-CF36-4C6E-982A-7CD81721CBE8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{B10C88B5-93E7-4164-A8CA-16712C801F8B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2832" yWindow="0" windowWidth="22692" windowHeight="8748" activeTab="1" xr2:uid="{D283E0F8-1F52-4946-9F02-CCA289FF9208}"/>
+    <workbookView xWindow="3780" yWindow="0" windowWidth="22695" windowHeight="8745" activeTab="1" xr2:uid="{D283E0F8-1F52-4946-9F02-CCA289FF9208}"/>
   </bookViews>
   <sheets>
     <sheet name="runs" sheetId="2" r:id="rId1"/>
     <sheet name="params" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -440,15 +440,15 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -456,20 +456,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
       <c r="B2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3">
-        <v>500</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -482,22 +482,22 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J16"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -532,7 +532,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -543,10 +543,10 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F2">
         <v>270</v>
@@ -567,7 +567,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -602,7 +602,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -637,7 +637,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -672,7 +672,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -707,7 +707,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -742,7 +742,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -777,7 +777,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -812,7 +812,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -847,7 +847,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -882,7 +882,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -917,7 +917,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -952,7 +952,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -987,7 +987,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Save before changing branches
</commit_message>
<xml_diff>
--- a/AAE 560 Air Taxi Model/+airtaxi/Inputs.xlsx
+++ b/AAE 560 Air Taxi Model/+airtaxi/Inputs.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Documents\GitHub\SoS12\AAE 560 Air Taxi Model\+airtaxi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5411BE5-CF36-4C6E-982A-7CD81721CBE8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E1F8B59-81A6-4B45-9BFB-8C959F300785}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2832" yWindow="0" windowWidth="22692" windowHeight="8748" activeTab="1" xr2:uid="{D283E0F8-1F52-4946-9F02-CCA289FF9208}"/>
+    <workbookView xWindow="3780" yWindow="0" windowWidth="22692" windowHeight="8748" activeTab="1" xr2:uid="{D283E0F8-1F52-4946-9F02-CCA289FF9208}"/>
   </bookViews>
   <sheets>
     <sheet name="runs" sheetId="2" r:id="rId1"/>
     <sheet name="params" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -73,6 +73,9 @@
     <t>Stop Run ID (inclusive)</t>
   </si>
   <si>
+    <t>config5</t>
+  </si>
+  <si>
     <t>config2</t>
   </si>
   <si>
@@ -80,9 +83,6 @@
   </si>
   <si>
     <t>config4</t>
-  </si>
-  <si>
-    <t>config5</t>
   </si>
 </sst>
 </file>
@@ -440,7 +440,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -482,7 +482,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J16"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -543,7 +543,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -561,7 +561,7 @@
         <v>5</v>
       </c>
       <c r="J2">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="K2" t="s">
         <v>10</v>
@@ -596,10 +596,10 @@
         <v>5</v>
       </c>
       <c r="J3">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="K3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -631,10 +631,10 @@
         <v>5</v>
       </c>
       <c r="J4">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="K4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -666,10 +666,10 @@
         <v>5</v>
       </c>
       <c r="J5">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="K5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -683,7 +683,7 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="E6">
         <v>3</v>
@@ -701,10 +701,10 @@
         <v>5</v>
       </c>
       <c r="J6">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="K6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -712,7 +712,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <v>10</v>
@@ -736,7 +736,7 @@
         <v>5</v>
       </c>
       <c r="J7">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="K7" t="s">
         <v>10</v>
@@ -747,10 +747,10 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C8">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D8">
         <v>0.9</v>
@@ -771,10 +771,10 @@
         <v>5</v>
       </c>
       <c r="J8">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="K8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -782,10 +782,10 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C9">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="D9">
         <v>0.8</v>
@@ -806,10 +806,10 @@
         <v>5</v>
       </c>
       <c r="J9">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="K9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -817,10 +817,10 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="C10">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="D10">
         <v>0.7</v>
@@ -841,10 +841,10 @@
         <v>5</v>
       </c>
       <c r="J10">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="K10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -852,13 +852,13 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="C11">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="E11">
         <v>3</v>
@@ -876,10 +876,10 @@
         <v>5</v>
       </c>
       <c r="J11">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="K11" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -890,7 +890,7 @@
         <v>10</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -911,7 +911,7 @@
         <v>5</v>
       </c>
       <c r="J12">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="K12" t="s">
         <v>10</v>
@@ -922,7 +922,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C13">
         <v>10</v>
@@ -946,10 +946,10 @@
         <v>5</v>
       </c>
       <c r="J13">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="K13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -957,10 +957,10 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C14">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D14">
         <v>0.8</v>
@@ -981,10 +981,10 @@
         <v>5</v>
       </c>
       <c r="J14">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="K14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -992,10 +992,10 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C15">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D15">
         <v>0.7</v>
@@ -1016,10 +1016,10 @@
         <v>5</v>
       </c>
       <c r="J15">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="K15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -1027,13 +1027,13 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="C16">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="E16">
         <v>3</v>
@@ -1051,10 +1051,10 @@
         <v>5</v>
       </c>
       <c r="J16">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="K16" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Divided by speed scale factor before inputting to pdf
</commit_message>
<xml_diff>
--- a/AAE 560 Air Taxi Model/+airtaxi/Inputs.xlsx
+++ b/AAE 560 Air Taxi Model/+airtaxi/Inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Documents\GitHub\SoS12\AAE 560 Air Taxi Model\+airtaxi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E1F8B59-81A6-4B45-9BFB-8C959F300785}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB6D82D-CC60-4D0A-8141-E1F27CB42EF5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3780" yWindow="0" windowWidth="22692" windowHeight="8748" activeTab="1" xr2:uid="{D283E0F8-1F52-4946-9F02-CCA289FF9208}"/>
   </bookViews>
@@ -440,7 +440,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -469,7 +469,7 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>500</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -482,7 +482,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Fixed bug in equation
</commit_message>
<xml_diff>
--- a/AAE 560 Air Taxi Model/+airtaxi/Inputs.xlsx
+++ b/AAE 560 Air Taxi Model/+airtaxi/Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Documents\GitHub\SoS12\AAE 560 Air Taxi Model\+airtaxi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB6D82D-CC60-4D0A-8141-E1F27CB42EF5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B655B29-8F41-46E1-85F9-372E4E8E4119}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="0" windowWidth="22692" windowHeight="8748" activeTab="1" xr2:uid="{D283E0F8-1F52-4946-9F02-CCA289FF9208}"/>
+    <workbookView xWindow="3780" yWindow="0" windowWidth="22692" windowHeight="8748" xr2:uid="{D283E0F8-1F52-4946-9F02-CCA289FF9208}"/>
   </bookViews>
   <sheets>
     <sheet name="runs" sheetId="2" r:id="rId1"/>
@@ -439,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98028C58-071A-4E37-9E82-3C2AA620C0F8}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -461,7 +461,7 @@
         <v>14</v>
       </c>
       <c r="B2">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -481,7 +481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD319FC3-F5A0-442C-9F04-E5E568694E63}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Made changes to calculated expected values
Now our model is officially stochastic!
</commit_message>
<xml_diff>
--- a/AAE 560 Air Taxi Model/+airtaxi/Inputs.xlsx
+++ b/AAE 560 Air Taxi Model/+airtaxi/Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Documents\GitHub\SoS12\AAE 560 Air Taxi Model\+airtaxi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF71612-3BA7-47DF-8134-1DC8ED2E56AA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5E24BE-CE72-46DE-90FA-DE4CA681BEC2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="0" windowWidth="22692" windowHeight="8748" activeTab="1" xr2:uid="{D283E0F8-1F52-4946-9F02-CCA289FF9208}"/>
+    <workbookView xWindow="3780" yWindow="0" windowWidth="22692" windowHeight="8748" xr2:uid="{D283E0F8-1F52-4946-9F02-CCA289FF9208}"/>
   </bookViews>
   <sheets>
     <sheet name="runs" sheetId="2" r:id="rId1"/>
@@ -430,8 +430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98028C58-071A-4E37-9E82-3C2AA620C0F8}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -452,7 +452,7 @@
         <v>14</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -472,7 +472,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD319FC3-F5A0-442C-9F04-E5E568694E63}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Minor adjustment to crash_threshold
</commit_message>
<xml_diff>
--- a/AAE 560 Air Taxi Model/+airtaxi/Inputs.xlsx
+++ b/AAE 560 Air Taxi Model/+airtaxi/Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Documents\GitHub\SoS12\AAE 560 Air Taxi Model\+airtaxi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5E24BE-CE72-46DE-90FA-DE4CA681BEC2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1422A7FA-B8ED-4646-9242-6DD3A4F31798}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="0" windowWidth="22692" windowHeight="8748" xr2:uid="{D283E0F8-1F52-4946-9F02-CCA289FF9208}"/>
+    <workbookView xWindow="3780" yWindow="0" windowWidth="22692" windowHeight="8748" activeTab="1" xr2:uid="{D283E0F8-1F52-4946-9F02-CCA289FF9208}"/>
   </bookViews>
   <sheets>
     <sheet name="runs" sheetId="2" r:id="rId1"/>
@@ -430,7 +430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98028C58-071A-4E37-9E82-3C2AA620C0F8}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -452,7 +452,7 @@
         <v>14</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -460,7 +460,7 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>100</v>
+        <v>500</v>
       </c>
     </row>
   </sheetData>
@@ -472,8 +472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD319FC3-F5A0-442C-9F04-E5E568694E63}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -552,7 +552,7 @@
         <v>5</v>
       </c>
       <c r="J2">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="K2" t="s">
         <v>15</v>
@@ -587,7 +587,7 @@
         <v>5</v>
       </c>
       <c r="J3">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="K3" t="s">
         <v>10</v>
@@ -622,7 +622,7 @@
         <v>5</v>
       </c>
       <c r="J4">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="K4" t="s">
         <v>10</v>
@@ -657,7 +657,7 @@
         <v>5</v>
       </c>
       <c r="J5">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="K5" t="s">
         <v>10</v>
@@ -692,7 +692,7 @@
         <v>5</v>
       </c>
       <c r="J6">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="K6" t="s">
         <v>10</v>
@@ -727,7 +727,7 @@
         <v>5</v>
       </c>
       <c r="J7">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="K7" t="s">
         <v>10</v>
@@ -762,7 +762,7 @@
         <v>5</v>
       </c>
       <c r="J8">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="K8" t="s">
         <v>10</v>
@@ -797,7 +797,7 @@
         <v>5</v>
       </c>
       <c r="J9">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="K9" t="s">
         <v>10</v>
@@ -832,7 +832,7 @@
         <v>5</v>
       </c>
       <c r="J10">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="K10" t="s">
         <v>10</v>
@@ -867,7 +867,7 @@
         <v>5</v>
       </c>
       <c r="J11">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="K11" t="s">
         <v>10</v>
@@ -902,7 +902,7 @@
         <v>5</v>
       </c>
       <c r="J12">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="K12" t="s">
         <v>10</v>
@@ -937,7 +937,7 @@
         <v>5</v>
       </c>
       <c r="J13">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="K13" t="s">
         <v>10</v>
@@ -972,7 +972,7 @@
         <v>5</v>
       </c>
       <c r="J14">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="K14" t="s">
         <v>10</v>
@@ -1007,7 +1007,7 @@
         <v>5</v>
       </c>
       <c r="J15">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="K15" t="s">
         <v>10</v>
@@ -1042,7 +1042,7 @@
         <v>5</v>
       </c>
       <c r="J16">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="K16" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Everything is debugged - no more plot problems
</commit_message>
<xml_diff>
--- a/AAE 560 Air Taxi Model/+airtaxi/Inputs.xlsx
+++ b/AAE 560 Air Taxi Model/+airtaxi/Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Documents\GitHub\SoS12\AAE 560 Air Taxi Model\+airtaxi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6036C76-7505-4043-B22A-60FA194AFD21}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D0308B7-6C7E-4ABE-9222-FC9CACB95DA4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="0" windowWidth="22692" windowHeight="8748" xr2:uid="{D283E0F8-1F52-4946-9F02-CCA289FF9208}"/>
+    <workbookView xWindow="3780" yWindow="0" windowWidth="22692" windowHeight="8748" activeTab="1" xr2:uid="{D283E0F8-1F52-4946-9F02-CCA289FF9208}"/>
   </bookViews>
   <sheets>
     <sheet name="runs" sheetId="2" r:id="rId1"/>
@@ -430,7 +430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98028C58-071A-4E37-9E82-3C2AA620C0F8}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -472,8 +472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD319FC3-F5A0-442C-9F04-E5E568694E63}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -534,7 +534,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <v>3</v>

</xml_diff>

<commit_message>
Change the plot label to "km"
</commit_message>
<xml_diff>
--- a/AAE 560 Air Taxi Model/+airtaxi/Inputs.xlsx
+++ b/AAE 560 Air Taxi Model/+airtaxi/Inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chenr\Documents\GitHub\SoS12\AAE 560 Air Taxi Model\+airtaxi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5151C0E6-1E09-464C-9842-1014EB5E935C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFBE706-BCC2-42AD-AA28-D23E7DF58BB3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3780" yWindow="0" windowWidth="22692" windowHeight="8748" activeTab="1" xr2:uid="{D283E0F8-1F52-4946-9F02-CCA289FF9208}"/>
   </bookViews>
@@ -431,7 +431,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -452,7 +452,7 @@
         <v>14</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -473,7 +473,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J16"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Final Input File Update
Get rid of the first 15 runs and shift everything up.
</commit_message>
<xml_diff>
--- a/AAE 560 Air Taxi Model/+airtaxi/Inputs.xlsx
+++ b/AAE 560 Air Taxi Model/+airtaxi/Inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chenr\Documents\GitHub\SoS12\AAE 560 Air Taxi Model\+airtaxi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D30014DC-6EE7-4C62-A24B-A6731344EAC4}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6EAD9B-9070-4F6B-B3F8-7116C8EC46BD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7668" activeTab="1" xr2:uid="{D283E0F8-1F52-4946-9F02-CCA289FF9208}"/>
   </bookViews>
@@ -518,10 +518,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD319FC3-F5A0-442C-9F04-E5E568694E63}">
-  <dimension ref="A1:L1267"/>
+  <dimension ref="A1:L1041"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A942" sqref="A942:A1041"/>
+      <selection activeCell="A1058" sqref="A1058:A1267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -37001,1056 +37001,6 @@
         <v>15</v>
       </c>
     </row>
-    <row r="1058" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1058">
-        <v>1057</v>
-      </c>
-    </row>
-    <row r="1059" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1059">
-        <v>1058</v>
-      </c>
-    </row>
-    <row r="1060" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1060">
-        <v>1059</v>
-      </c>
-    </row>
-    <row r="1061" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1061">
-        <v>1060</v>
-      </c>
-    </row>
-    <row r="1062" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1062">
-        <v>1061</v>
-      </c>
-    </row>
-    <row r="1063" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1063">
-        <v>1062</v>
-      </c>
-    </row>
-    <row r="1064" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1064">
-        <v>1063</v>
-      </c>
-    </row>
-    <row r="1065" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1065">
-        <v>1064</v>
-      </c>
-    </row>
-    <row r="1066" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1066">
-        <v>1065</v>
-      </c>
-    </row>
-    <row r="1067" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1067">
-        <v>1066</v>
-      </c>
-    </row>
-    <row r="1068" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1068">
-        <v>1067</v>
-      </c>
-    </row>
-    <row r="1069" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1069">
-        <v>1068</v>
-      </c>
-    </row>
-    <row r="1070" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1070">
-        <v>1069</v>
-      </c>
-    </row>
-    <row r="1071" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1071">
-        <v>1070</v>
-      </c>
-    </row>
-    <row r="1072" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1072">
-        <v>1071</v>
-      </c>
-    </row>
-    <row r="1073" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1073">
-        <v>1072</v>
-      </c>
-    </row>
-    <row r="1074" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1074">
-        <v>1073</v>
-      </c>
-    </row>
-    <row r="1075" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1075">
-        <v>1074</v>
-      </c>
-    </row>
-    <row r="1076" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1076">
-        <v>1075</v>
-      </c>
-    </row>
-    <row r="1077" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1077">
-        <v>1076</v>
-      </c>
-    </row>
-    <row r="1078" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1078">
-        <v>1077</v>
-      </c>
-    </row>
-    <row r="1079" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1079">
-        <v>1078</v>
-      </c>
-    </row>
-    <row r="1080" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1080">
-        <v>1079</v>
-      </c>
-    </row>
-    <row r="1081" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1081">
-        <v>1080</v>
-      </c>
-    </row>
-    <row r="1082" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1082">
-        <v>1081</v>
-      </c>
-    </row>
-    <row r="1083" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1083">
-        <v>1082</v>
-      </c>
-    </row>
-    <row r="1084" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1084">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="1085" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1085">
-        <v>1084</v>
-      </c>
-    </row>
-    <row r="1086" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1086">
-        <v>1085</v>
-      </c>
-    </row>
-    <row r="1087" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1087">
-        <v>1086</v>
-      </c>
-    </row>
-    <row r="1088" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1088">
-        <v>1087</v>
-      </c>
-    </row>
-    <row r="1089" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1089">
-        <v>1088</v>
-      </c>
-    </row>
-    <row r="1090" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1090">
-        <v>1089</v>
-      </c>
-    </row>
-    <row r="1091" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1091">
-        <v>1090</v>
-      </c>
-    </row>
-    <row r="1092" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1092">
-        <v>1091</v>
-      </c>
-    </row>
-    <row r="1093" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1093">
-        <v>1092</v>
-      </c>
-    </row>
-    <row r="1094" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1094">
-        <v>1093</v>
-      </c>
-    </row>
-    <row r="1095" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1095">
-        <v>1094</v>
-      </c>
-    </row>
-    <row r="1096" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1096">
-        <v>1095</v>
-      </c>
-    </row>
-    <row r="1097" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1097">
-        <v>1096</v>
-      </c>
-    </row>
-    <row r="1098" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1098">
-        <v>1097</v>
-      </c>
-    </row>
-    <row r="1099" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1099">
-        <v>1098</v>
-      </c>
-    </row>
-    <row r="1100" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1100">
-        <v>1099</v>
-      </c>
-    </row>
-    <row r="1101" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1101">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="1102" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1102">
-        <v>1101</v>
-      </c>
-    </row>
-    <row r="1103" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1103">
-        <v>1102</v>
-      </c>
-    </row>
-    <row r="1104" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1104">
-        <v>1103</v>
-      </c>
-    </row>
-    <row r="1105" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1105">
-        <v>1104</v>
-      </c>
-    </row>
-    <row r="1106" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1106">
-        <v>1105</v>
-      </c>
-    </row>
-    <row r="1107" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1107">
-        <v>1106</v>
-      </c>
-    </row>
-    <row r="1108" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1108">
-        <v>1107</v>
-      </c>
-    </row>
-    <row r="1109" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1109">
-        <v>1108</v>
-      </c>
-    </row>
-    <row r="1110" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1110">
-        <v>1109</v>
-      </c>
-    </row>
-    <row r="1111" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1111">
-        <v>1110</v>
-      </c>
-    </row>
-    <row r="1112" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1112">
-        <v>1111</v>
-      </c>
-    </row>
-    <row r="1113" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1113">
-        <v>1112</v>
-      </c>
-    </row>
-    <row r="1114" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1114">
-        <v>1113</v>
-      </c>
-    </row>
-    <row r="1115" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1115">
-        <v>1114</v>
-      </c>
-    </row>
-    <row r="1116" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1116">
-        <v>1115</v>
-      </c>
-    </row>
-    <row r="1117" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1117">
-        <v>1116</v>
-      </c>
-    </row>
-    <row r="1118" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1118">
-        <v>1117</v>
-      </c>
-    </row>
-    <row r="1119" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1119">
-        <v>1118</v>
-      </c>
-    </row>
-    <row r="1120" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1120">
-        <v>1119</v>
-      </c>
-    </row>
-    <row r="1121" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1121">
-        <v>1120</v>
-      </c>
-    </row>
-    <row r="1122" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1122">
-        <v>1121</v>
-      </c>
-    </row>
-    <row r="1123" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1123">
-        <v>1122</v>
-      </c>
-    </row>
-    <row r="1124" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1124">
-        <v>1123</v>
-      </c>
-    </row>
-    <row r="1125" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1125">
-        <v>1124</v>
-      </c>
-    </row>
-    <row r="1126" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1126">
-        <v>1125</v>
-      </c>
-    </row>
-    <row r="1127" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1127">
-        <v>1126</v>
-      </c>
-    </row>
-    <row r="1128" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1128">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="1129" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1129">
-        <v>1128</v>
-      </c>
-    </row>
-    <row r="1130" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1130">
-        <v>1129</v>
-      </c>
-    </row>
-    <row r="1131" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1131">
-        <v>1130</v>
-      </c>
-    </row>
-    <row r="1132" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1132">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="1133" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1133">
-        <v>1132</v>
-      </c>
-    </row>
-    <row r="1134" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1134">
-        <v>1133</v>
-      </c>
-    </row>
-    <row r="1135" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1135">
-        <v>1134</v>
-      </c>
-    </row>
-    <row r="1136" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1136">
-        <v>1135</v>
-      </c>
-    </row>
-    <row r="1137" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1137">
-        <v>1136</v>
-      </c>
-    </row>
-    <row r="1138" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1138">
-        <v>1137</v>
-      </c>
-    </row>
-    <row r="1139" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1139">
-        <v>1138</v>
-      </c>
-    </row>
-    <row r="1140" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1140">
-        <v>1139</v>
-      </c>
-    </row>
-    <row r="1141" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1141">
-        <v>1140</v>
-      </c>
-    </row>
-    <row r="1142" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1142">
-        <v>1141</v>
-      </c>
-    </row>
-    <row r="1143" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1143">
-        <v>1142</v>
-      </c>
-    </row>
-    <row r="1144" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1144">
-        <v>1143</v>
-      </c>
-    </row>
-    <row r="1145" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1145">
-        <v>1144</v>
-      </c>
-    </row>
-    <row r="1146" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1146">
-        <v>1145</v>
-      </c>
-    </row>
-    <row r="1147" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1147">
-        <v>1146</v>
-      </c>
-    </row>
-    <row r="1148" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1148">
-        <v>1147</v>
-      </c>
-    </row>
-    <row r="1149" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1149">
-        <v>1148</v>
-      </c>
-    </row>
-    <row r="1150" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1150">
-        <v>1149</v>
-      </c>
-    </row>
-    <row r="1151" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1151">
-        <v>1150</v>
-      </c>
-    </row>
-    <row r="1152" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1152">
-        <v>1151</v>
-      </c>
-    </row>
-    <row r="1153" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1153">
-        <v>1152</v>
-      </c>
-    </row>
-    <row r="1154" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1154">
-        <v>1153</v>
-      </c>
-    </row>
-    <row r="1155" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1155">
-        <v>1154</v>
-      </c>
-    </row>
-    <row r="1156" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1156">
-        <v>1155</v>
-      </c>
-    </row>
-    <row r="1157" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1157">
-        <v>1156</v>
-      </c>
-    </row>
-    <row r="1158" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1158">
-        <v>1157</v>
-      </c>
-    </row>
-    <row r="1159" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1159">
-        <v>1158</v>
-      </c>
-    </row>
-    <row r="1160" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1160">
-        <v>1159</v>
-      </c>
-    </row>
-    <row r="1161" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1161">
-        <v>1160</v>
-      </c>
-    </row>
-    <row r="1162" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1162">
-        <v>1161</v>
-      </c>
-    </row>
-    <row r="1163" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1163">
-        <v>1162</v>
-      </c>
-    </row>
-    <row r="1164" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1164">
-        <v>1163</v>
-      </c>
-    </row>
-    <row r="1165" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1165">
-        <v>1164</v>
-      </c>
-    </row>
-    <row r="1166" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1166">
-        <v>1165</v>
-      </c>
-    </row>
-    <row r="1167" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1167">
-        <v>1166</v>
-      </c>
-    </row>
-    <row r="1168" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1168">
-        <v>1167</v>
-      </c>
-    </row>
-    <row r="1169" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1169">
-        <v>1168</v>
-      </c>
-    </row>
-    <row r="1170" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1170">
-        <v>1169</v>
-      </c>
-    </row>
-    <row r="1171" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1171">
-        <v>1170</v>
-      </c>
-    </row>
-    <row r="1172" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1172">
-        <v>1171</v>
-      </c>
-    </row>
-    <row r="1173" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1173">
-        <v>1172</v>
-      </c>
-    </row>
-    <row r="1174" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1174">
-        <v>1173</v>
-      </c>
-    </row>
-    <row r="1175" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1175">
-        <v>1174</v>
-      </c>
-    </row>
-    <row r="1176" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1176">
-        <v>1175</v>
-      </c>
-    </row>
-    <row r="1177" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1177">
-        <v>1176</v>
-      </c>
-    </row>
-    <row r="1178" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1178">
-        <v>1177</v>
-      </c>
-    </row>
-    <row r="1179" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1179">
-        <v>1178</v>
-      </c>
-    </row>
-    <row r="1180" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1180">
-        <v>1179</v>
-      </c>
-    </row>
-    <row r="1181" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1181">
-        <v>1180</v>
-      </c>
-    </row>
-    <row r="1182" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1182">
-        <v>1181</v>
-      </c>
-    </row>
-    <row r="1183" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1183">
-        <v>1182</v>
-      </c>
-    </row>
-    <row r="1184" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1184">
-        <v>1183</v>
-      </c>
-    </row>
-    <row r="1185" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1185">
-        <v>1184</v>
-      </c>
-    </row>
-    <row r="1186" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1186">
-        <v>1185</v>
-      </c>
-    </row>
-    <row r="1187" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1187">
-        <v>1186</v>
-      </c>
-    </row>
-    <row r="1188" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1188">
-        <v>1187</v>
-      </c>
-    </row>
-    <row r="1189" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1189">
-        <v>1188</v>
-      </c>
-    </row>
-    <row r="1190" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1190">
-        <v>1189</v>
-      </c>
-    </row>
-    <row r="1191" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1191">
-        <v>1190</v>
-      </c>
-    </row>
-    <row r="1192" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1192">
-        <v>1191</v>
-      </c>
-    </row>
-    <row r="1193" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1193">
-        <v>1192</v>
-      </c>
-    </row>
-    <row r="1194" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1194">
-        <v>1193</v>
-      </c>
-    </row>
-    <row r="1195" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1195">
-        <v>1194</v>
-      </c>
-    </row>
-    <row r="1196" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1196">
-        <v>1195</v>
-      </c>
-    </row>
-    <row r="1197" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1197">
-        <v>1196</v>
-      </c>
-    </row>
-    <row r="1198" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1198">
-        <v>1197</v>
-      </c>
-    </row>
-    <row r="1199" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1199">
-        <v>1198</v>
-      </c>
-    </row>
-    <row r="1200" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1200">
-        <v>1199</v>
-      </c>
-    </row>
-    <row r="1201" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1201">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="1202" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1202">
-        <v>1201</v>
-      </c>
-    </row>
-    <row r="1203" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1203">
-        <v>1202</v>
-      </c>
-    </row>
-    <row r="1204" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1204">
-        <v>1203</v>
-      </c>
-    </row>
-    <row r="1205" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1205">
-        <v>1204</v>
-      </c>
-    </row>
-    <row r="1206" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1206">
-        <v>1205</v>
-      </c>
-    </row>
-    <row r="1207" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1207">
-        <v>1206</v>
-      </c>
-    </row>
-    <row r="1208" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1208">
-        <v>1207</v>
-      </c>
-    </row>
-    <row r="1209" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1209">
-        <v>1208</v>
-      </c>
-    </row>
-    <row r="1210" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1210">
-        <v>1209</v>
-      </c>
-    </row>
-    <row r="1211" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1211">
-        <v>1210</v>
-      </c>
-    </row>
-    <row r="1212" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1212">
-        <v>1211</v>
-      </c>
-    </row>
-    <row r="1213" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1213">
-        <v>1212</v>
-      </c>
-    </row>
-    <row r="1214" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1214">
-        <v>1213</v>
-      </c>
-    </row>
-    <row r="1215" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1215">
-        <v>1214</v>
-      </c>
-    </row>
-    <row r="1216" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1216">
-        <v>1215</v>
-      </c>
-    </row>
-    <row r="1217" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1217">
-        <v>1216</v>
-      </c>
-    </row>
-    <row r="1218" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1218">
-        <v>1217</v>
-      </c>
-    </row>
-    <row r="1219" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1219">
-        <v>1218</v>
-      </c>
-    </row>
-    <row r="1220" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1220">
-        <v>1219</v>
-      </c>
-    </row>
-    <row r="1221" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1221">
-        <v>1220</v>
-      </c>
-    </row>
-    <row r="1222" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1222">
-        <v>1221</v>
-      </c>
-    </row>
-    <row r="1223" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1223">
-        <v>1222</v>
-      </c>
-    </row>
-    <row r="1224" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1224">
-        <v>1223</v>
-      </c>
-    </row>
-    <row r="1225" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1225">
-        <v>1224</v>
-      </c>
-    </row>
-    <row r="1226" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1226">
-        <v>1225</v>
-      </c>
-    </row>
-    <row r="1227" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1227">
-        <v>1226</v>
-      </c>
-    </row>
-    <row r="1228" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1228">
-        <v>1227</v>
-      </c>
-    </row>
-    <row r="1229" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1229">
-        <v>1228</v>
-      </c>
-    </row>
-    <row r="1230" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1230">
-        <v>1229</v>
-      </c>
-    </row>
-    <row r="1231" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1231">
-        <v>1230</v>
-      </c>
-    </row>
-    <row r="1232" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1232">
-        <v>1231</v>
-      </c>
-    </row>
-    <row r="1233" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1233">
-        <v>1232</v>
-      </c>
-    </row>
-    <row r="1234" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1234">
-        <v>1233</v>
-      </c>
-    </row>
-    <row r="1235" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1235">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="1236" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1236">
-        <v>1235</v>
-      </c>
-    </row>
-    <row r="1237" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1237">
-        <v>1236</v>
-      </c>
-    </row>
-    <row r="1238" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1238">
-        <v>1237</v>
-      </c>
-    </row>
-    <row r="1239" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1239">
-        <v>1238</v>
-      </c>
-    </row>
-    <row r="1240" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1240">
-        <v>1239</v>
-      </c>
-    </row>
-    <row r="1241" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1241">
-        <v>1240</v>
-      </c>
-    </row>
-    <row r="1242" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1242">
-        <v>1241</v>
-      </c>
-    </row>
-    <row r="1243" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1243">
-        <v>1242</v>
-      </c>
-    </row>
-    <row r="1244" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1244">
-        <v>1243</v>
-      </c>
-    </row>
-    <row r="1245" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1245">
-        <v>1244</v>
-      </c>
-    </row>
-    <row r="1246" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1246">
-        <v>1245</v>
-      </c>
-    </row>
-    <row r="1247" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1247">
-        <v>1246</v>
-      </c>
-    </row>
-    <row r="1248" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1248">
-        <v>1247</v>
-      </c>
-    </row>
-    <row r="1249" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1249">
-        <v>1248</v>
-      </c>
-    </row>
-    <row r="1250" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1250">
-        <v>1249</v>
-      </c>
-    </row>
-    <row r="1251" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1251">
-        <v>1250</v>
-      </c>
-    </row>
-    <row r="1252" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1252">
-        <v>1251</v>
-      </c>
-    </row>
-    <row r="1253" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1253">
-        <v>1252</v>
-      </c>
-    </row>
-    <row r="1254" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1254">
-        <v>1253</v>
-      </c>
-    </row>
-    <row r="1255" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1255">
-        <v>1254</v>
-      </c>
-    </row>
-    <row r="1256" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1256">
-        <v>1255</v>
-      </c>
-    </row>
-    <row r="1257" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1257">
-        <v>1256</v>
-      </c>
-    </row>
-    <row r="1258" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1258">
-        <v>1257</v>
-      </c>
-    </row>
-    <row r="1259" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1259">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="1260" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1260">
-        <v>1259</v>
-      </c>
-    </row>
-    <row r="1261" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1261">
-        <v>1260</v>
-      </c>
-    </row>
-    <row r="1262" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1262">
-        <v>1261</v>
-      </c>
-    </row>
-    <row r="1263" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1263">
-        <v>1262</v>
-      </c>
-    </row>
-    <row r="1264" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1264">
-        <v>1263</v>
-      </c>
-    </row>
-    <row r="1265" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1265">
-        <v>1264</v>
-      </c>
-    </row>
-    <row r="1266" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1266">
-        <v>1265</v>
-      </c>
-    </row>
-    <row r="1267" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1267">
-        <v>1266</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>

</xml_diff>